<commit_message>
Start mop activity bill parser - CoP error
</commit_message>
<xml_diff>
--- a/test/electricity/bills.activity.mop.stark.xlsx
+++ b/test/electricity/bills.activity.mop.stark.xlsx
@@ -134,7 +134,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -152,6 +152,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -201,14 +205,14 @@
   <dimension ref="B6:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.37"/>
@@ -275,7 +279,9 @@
       <c r="B13" s="3" t="n">
         <v>1472066139971</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="5" t="n">
+        <v>5</v>
+      </c>
       <c r="D13" s="0" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Add VAT and gross to activity.mop.stark.xlsx parser
</commit_message>
<xml_diff>
--- a/test/electricity/bills.activity.mop.stark.xlsx
+++ b/test/electricity/bills.activity.mop.stark.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">Invoice Date</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t xml:space="preserve">Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross</t>
   </si>
   <si>
     <t xml:space="preserve">Settled</t>
@@ -134,7 +140,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -152,10 +158,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -202,10 +204,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B6:I13"/>
+  <dimension ref="B6:K13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -253,6 +255,12 @@
       <c r="I11" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="J11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="n">
@@ -260,42 +268,54 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F12" s="4" t="n">
         <v>43252</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>135.81</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>13.53</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>150.56</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="n">
         <v>1472066139971</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>29738</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>135.81</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>13.53</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>150.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>